<commit_message>
Fixing names to match
</commit_message>
<xml_diff>
--- a/assets/Combined_Daily_Data.xlsx
+++ b/assets/Combined_Daily_Data.xlsx
@@ -541,15 +541,6 @@
     <t>Trea Turner</t>
   </si>
   <si>
-    <t>Bryce Harper</t>
-  </si>
-  <si>
-    <t>David Dahl</t>
-  </si>
-  <si>
-    <t>Kyle Schwarber</t>
-  </si>
-  <si>
     <t>Garrett Stubbs</t>
   </si>
   <si>
@@ -559,12 +550,21 @@
     <t>Alec Bohm</t>
   </si>
   <si>
+    <t>Whit Merrifield</t>
+  </si>
+  <si>
     <t>Brandon Marsh</t>
   </si>
   <si>
     <t>Bryson Stott</t>
   </si>
   <si>
+    <t>Kody Clemens</t>
+  </si>
+  <si>
+    <t>Johan Rojas</t>
+  </si>
+  <si>
     <t>Paul DeJong</t>
   </si>
   <si>
@@ -703,6 +703,9 @@
     <t>Jake Cave</t>
   </si>
   <si>
+    <t>Sam Hilliard</t>
+  </si>
+  <si>
     <t>Jacob Stallings</t>
   </si>
   <si>
@@ -724,9 +727,6 @@
     <t>Nolan Jones</t>
   </si>
   <si>
-    <t>Hunter Goodman</t>
-  </si>
-  <si>
     <t>Anthony Santander</t>
   </si>
   <si>
@@ -823,9 +823,6 @@
     <t>Masataka Yoshida</t>
   </si>
   <si>
-    <t>Enmanuel Valdez</t>
-  </si>
-  <si>
     <t>Connor Wong</t>
   </si>
   <si>
@@ -833,6 +830,9 @@
   </si>
   <si>
     <t>Wilyer Abreu</t>
+  </si>
+  <si>
+    <t>Ceddanne Rafaela</t>
   </si>
   <si>
     <t>Michael Conforto</t>
@@ -19019,7 +19019,7 @@
         <v>378</v>
       </c>
       <c r="G120">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H120">
         <v>14</v>
@@ -19895,7 +19895,7 @@
         <v>378</v>
       </c>
       <c r="G126">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H126">
         <v>47</v>
@@ -20333,52 +20333,52 @@
         <v>377</v>
       </c>
       <c r="G129">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H129">
-        <v>174</v>
+        <v>55</v>
       </c>
       <c r="I129">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J129">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K129">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L129">
-        <v>0.299</v>
+        <v>0.2</v>
       </c>
       <c r="M129">
-        <v>0.407</v>
+        <v>0.219</v>
       </c>
       <c r="N129">
-        <v>0.276</v>
+        <v>0.018</v>
       </c>
       <c r="O129">
-        <v>0.397</v>
+        <v>0.254</v>
       </c>
       <c r="P129">
-        <v>0.575</v>
+        <v>0.218</v>
       </c>
       <c r="Q129">
-        <v>0.972</v>
+        <v>0.472</v>
       </c>
       <c r="R129">
-        <v>18.6</v>
+        <v>30.5</v>
       </c>
       <c r="S129">
-        <v>14.2</v>
+        <v>6.8</v>
       </c>
       <c r="T129">
-        <v>37.2</v>
+        <v>36.1</v>
       </c>
       <c r="U129">
-        <v>40.9</v>
+        <v>36.1</v>
       </c>
       <c r="V129">
-        <v>42.3</v>
+        <v>13.5</v>
       </c>
       <c r="W129" t="s">
         <v>393</v>
@@ -20441,22 +20441,22 @@
         <v>0.286</v>
       </c>
       <c r="AQ129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS129">
         <v>0</v>
       </c>
       <c r="AT129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV129">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:48">
@@ -20473,58 +20473,58 @@
         <v>176</v>
       </c>
       <c r="E130" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F130" t="s">
         <v>377</v>
       </c>
       <c r="G130">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H130">
-        <v>38</v>
+        <v>224</v>
       </c>
       <c r="I130">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K130">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L130">
-        <v>0.263</v>
+        <v>0.223</v>
       </c>
       <c r="M130">
-        <v>0.364</v>
+        <v>0.285</v>
       </c>
       <c r="N130">
-        <v>0.289</v>
+        <v>0.134</v>
       </c>
       <c r="O130">
-        <v>0.3</v>
+        <v>0.286</v>
       </c>
       <c r="P130">
-        <v>0.553</v>
+        <v>0.357</v>
       </c>
       <c r="Q130">
-        <v>0.853</v>
+        <v>0.643</v>
       </c>
       <c r="R130">
-        <v>20</v>
+        <v>20.4</v>
       </c>
       <c r="S130">
-        <v>5</v>
+        <v>6.9</v>
       </c>
       <c r="T130">
-        <v>43.3</v>
+        <v>38.9</v>
       </c>
       <c r="U130">
-        <v>40</v>
+        <v>38.3</v>
       </c>
       <c r="V130">
-        <v>40</v>
+        <v>29.7</v>
       </c>
       <c r="W130" t="s">
         <v>393</v>
@@ -20542,49 +20542,49 @@
         <v>393</v>
       </c>
       <c r="AB130" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC130">
         <v>12</v>
       </c>
       <c r="AD130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE130">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="AF130">
-        <v>0.436</v>
+        <v>0.192</v>
       </c>
       <c r="AG130">
-        <v>8.300000000000001</v>
+        <v>0</v>
       </c>
       <c r="AH130">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AI130">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="AJ130">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AK130">
-        <v>0.167</v>
+        <v>0.083</v>
       </c>
       <c r="AL130">
-        <v>8.029999999999999</v>
+        <v>4.96</v>
       </c>
       <c r="AM130">
-        <v>0.5710000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="AN130">
-        <v>0.286</v>
+        <v>0.2</v>
       </c>
       <c r="AO130">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AP130">
-        <v>0.286</v>
+        <v>0.2</v>
       </c>
       <c r="AQ130">
         <v>0</v>
@@ -20596,13 +20596,13 @@
         <v>0</v>
       </c>
       <c r="AT130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:48">
@@ -20619,58 +20619,58 @@
         <v>177</v>
       </c>
       <c r="E131" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F131" t="s">
         <v>377</v>
       </c>
       <c r="G131">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H131">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="I131">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J131">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L131">
-        <v>0.184</v>
+        <v>0.33</v>
       </c>
       <c r="M131">
-        <v>0.312</v>
+        <v>0.389</v>
       </c>
       <c r="N131">
-        <v>0.201</v>
+        <v>0.197</v>
       </c>
       <c r="O131">
-        <v>0.323</v>
+        <v>0.384</v>
       </c>
       <c r="P131">
-        <v>0.385</v>
+        <v>0.527</v>
       </c>
       <c r="Q131">
-        <v>0.708</v>
+        <v>0.911</v>
       </c>
       <c r="R131">
-        <v>29.5</v>
+        <v>14.8</v>
       </c>
       <c r="S131">
-        <v>16.6</v>
+        <v>7</v>
       </c>
       <c r="T131">
-        <v>37.4</v>
+        <v>42.5</v>
       </c>
       <c r="U131">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="V131">
-        <v>43.5</v>
+        <v>37.9</v>
       </c>
       <c r="W131" t="s">
         <v>393</v>
@@ -20688,64 +20688,64 @@
         <v>393</v>
       </c>
       <c r="AB131" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC131">
         <v>12</v>
       </c>
       <c r="AD131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE131">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="AF131">
-        <v>0.436</v>
+        <v>0.192</v>
       </c>
       <c r="AG131">
-        <v>8.300000000000001</v>
+        <v>0</v>
       </c>
       <c r="AH131">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AI131">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="AJ131">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AK131">
-        <v>0.167</v>
+        <v>0.083</v>
       </c>
       <c r="AL131">
-        <v>8.029999999999999</v>
+        <v>4.96</v>
       </c>
       <c r="AM131">
-        <v>0.5710000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="AN131">
-        <v>0.286</v>
+        <v>0.2</v>
       </c>
       <c r="AO131">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AP131">
-        <v>0.286</v>
+        <v>0.2</v>
       </c>
       <c r="AQ131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS131">
         <v>0</v>
       </c>
       <c r="AT131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV131">
         <v>1</v>
@@ -20765,58 +20765,58 @@
         <v>178</v>
       </c>
       <c r="E132" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F132" t="s">
         <v>377</v>
       </c>
       <c r="G132">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H132">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="I132">
         <v>0</v>
       </c>
       <c r="J132">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K132">
         <v>0</v>
       </c>
       <c r="L132">
-        <v>0.2</v>
+        <v>0.188</v>
       </c>
       <c r="M132">
+        <v>0.254</v>
+      </c>
+      <c r="N132">
+        <v>0.031</v>
+      </c>
+      <c r="O132">
+        <v>0.307</v>
+      </c>
+      <c r="P132">
         <v>0.219</v>
       </c>
-      <c r="N132">
-        <v>0.018</v>
-      </c>
-      <c r="O132">
-        <v>0.254</v>
-      </c>
-      <c r="P132">
-        <v>0.218</v>
-      </c>
       <c r="Q132">
-        <v>0.472</v>
+        <v>0.525</v>
       </c>
       <c r="R132">
-        <v>30.5</v>
+        <v>11.8</v>
       </c>
       <c r="S132">
-        <v>6.8</v>
+        <v>13.2</v>
       </c>
       <c r="T132">
-        <v>36.1</v>
+        <v>47.3</v>
       </c>
       <c r="U132">
-        <v>36.1</v>
+        <v>34.5</v>
       </c>
       <c r="V132">
-        <v>13.5</v>
+        <v>23.2</v>
       </c>
       <c r="W132" t="s">
         <v>393</v>
@@ -20834,58 +20834,58 @@
         <v>393</v>
       </c>
       <c r="AB132" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC132">
         <v>12</v>
       </c>
       <c r="AD132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE132">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="AF132">
-        <v>0.436</v>
+        <v>0.192</v>
       </c>
       <c r="AG132">
-        <v>8.300000000000001</v>
+        <v>0</v>
       </c>
       <c r="AH132">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AI132">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="AJ132">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AK132">
-        <v>0.167</v>
+        <v>0.083</v>
       </c>
       <c r="AL132">
-        <v>8.029999999999999</v>
+        <v>4.96</v>
       </c>
       <c r="AM132">
-        <v>0.5710000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="AN132">
-        <v>0.286</v>
+        <v>0.2</v>
       </c>
       <c r="AO132">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AP132">
-        <v>0.286</v>
+        <v>0.2</v>
       </c>
       <c r="AQ132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT132">
         <v>0</v>
@@ -20911,58 +20911,58 @@
         <v>179</v>
       </c>
       <c r="E133" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F133" t="s">
         <v>377</v>
       </c>
       <c r="G133">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H133">
-        <v>224</v>
+        <v>150</v>
       </c>
       <c r="I133">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J133">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K133">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L133">
-        <v>0.223</v>
+        <v>0.3</v>
       </c>
       <c r="M133">
-        <v>0.285</v>
+        <v>0.378</v>
       </c>
       <c r="N133">
-        <v>0.134</v>
+        <v>0.193</v>
       </c>
       <c r="O133">
-        <v>0.286</v>
+        <v>0.376</v>
       </c>
       <c r="P133">
-        <v>0.357</v>
+        <v>0.493</v>
       </c>
       <c r="Q133">
-        <v>0.643</v>
+        <v>0.87</v>
       </c>
       <c r="R133">
-        <v>20.4</v>
+        <v>27.1</v>
       </c>
       <c r="S133">
-        <v>6.9</v>
+        <v>11.2</v>
       </c>
       <c r="T133">
-        <v>38.9</v>
+        <v>35.2</v>
       </c>
       <c r="U133">
-        <v>38.3</v>
+        <v>34.3</v>
       </c>
       <c r="V133">
-        <v>29.7</v>
+        <v>41.9</v>
       </c>
       <c r="W133" t="s">
         <v>393</v>
@@ -20980,55 +20980,55 @@
         <v>393</v>
       </c>
       <c r="AB133" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AC133">
         <v>12</v>
       </c>
       <c r="AD133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE133">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AF133">
-        <v>0.192</v>
+        <v>0.436</v>
       </c>
       <c r="AG133">
-        <v>0</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="AH133">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AI133">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="AJ133">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AK133">
-        <v>0.083</v>
+        <v>0.167</v>
       </c>
       <c r="AL133">
-        <v>4.96</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="AM133">
-        <v>0.8</v>
+        <v>0.5710000000000001</v>
       </c>
       <c r="AN133">
-        <v>0.2</v>
+        <v>0.286</v>
       </c>
       <c r="AO133">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AP133">
-        <v>0.2</v>
+        <v>0.286</v>
       </c>
       <c r="AQ133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS133">
         <v>0</v>
@@ -21037,10 +21037,10 @@
         <v>0</v>
       </c>
       <c r="AU133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:48">
@@ -21057,58 +21057,58 @@
         <v>180</v>
       </c>
       <c r="E134" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F134" t="s">
         <v>377</v>
       </c>
       <c r="G134">
+        <v>1</v>
+      </c>
+      <c r="H134">
+        <v>181</v>
+      </c>
+      <c r="I134">
         <v>4</v>
       </c>
-      <c r="H134">
-        <v>203</v>
-      </c>
-      <c r="I134">
-        <v>6</v>
-      </c>
       <c r="J134">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="K134">
         <v>0</v>
       </c>
       <c r="L134">
-        <v>0.33</v>
+        <v>0.243</v>
       </c>
       <c r="M134">
-        <v>0.389</v>
+        <v>0.316</v>
       </c>
       <c r="N134">
-        <v>0.197</v>
+        <v>0.138</v>
       </c>
       <c r="O134">
-        <v>0.384</v>
+        <v>0.336</v>
       </c>
       <c r="P134">
-        <v>0.527</v>
+        <v>0.381</v>
       </c>
       <c r="Q134">
-        <v>0.911</v>
+        <v>0.718</v>
       </c>
       <c r="R134">
-        <v>14.8</v>
+        <v>14</v>
       </c>
       <c r="S134">
-        <v>7</v>
+        <v>12.1</v>
       </c>
       <c r="T134">
-        <v>42.5</v>
+        <v>43.2</v>
       </c>
       <c r="U134">
-        <v>31</v>
+        <v>38.1</v>
       </c>
       <c r="V134">
-        <v>37.9</v>
+        <v>28.8</v>
       </c>
       <c r="W134" t="s">
         <v>393</v>
@@ -21126,55 +21126,55 @@
         <v>393</v>
       </c>
       <c r="AB134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AC134">
         <v>12</v>
       </c>
       <c r="AD134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE134">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AF134">
-        <v>0.192</v>
+        <v>0.436</v>
       </c>
       <c r="AG134">
-        <v>0</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="AH134">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AI134">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="AJ134">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AK134">
-        <v>0.083</v>
+        <v>0.167</v>
       </c>
       <c r="AL134">
-        <v>4.96</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="AM134">
-        <v>0.8</v>
+        <v>0.5710000000000001</v>
       </c>
       <c r="AN134">
-        <v>0.2</v>
+        <v>0.286</v>
       </c>
       <c r="AO134">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AP134">
-        <v>0.2</v>
+        <v>0.286</v>
       </c>
       <c r="AQ134">
         <v>0</v>
       </c>
       <c r="AR134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS134">
         <v>0</v>
@@ -21183,10 +21183,10 @@
         <v>0</v>
       </c>
       <c r="AU134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:48">
@@ -21209,52 +21209,52 @@
         <v>377</v>
       </c>
       <c r="G135">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H135">
-        <v>150</v>
+        <v>34</v>
       </c>
       <c r="I135">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J135">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K135">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L135">
-        <v>0.3</v>
+        <v>0.265</v>
       </c>
       <c r="M135">
-        <v>0.378</v>
+        <v>0.391</v>
       </c>
       <c r="N135">
-        <v>0.193</v>
+        <v>0.382</v>
       </c>
       <c r="O135">
-        <v>0.376</v>
+        <v>0.286</v>
       </c>
       <c r="P135">
-        <v>0.493</v>
+        <v>0.647</v>
       </c>
       <c r="Q135">
-        <v>0.87</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="R135">
-        <v>27.1</v>
+        <v>25.7</v>
       </c>
       <c r="S135">
-        <v>11.2</v>
+        <v>2.9</v>
       </c>
       <c r="T135">
-        <v>35.2</v>
+        <v>40</v>
       </c>
       <c r="U135">
-        <v>34.3</v>
+        <v>48</v>
       </c>
       <c r="V135">
-        <v>41.9</v>
+        <v>48</v>
       </c>
       <c r="W135" t="s">
         <v>393</v>
@@ -21320,13 +21320,13 @@
         <v>1</v>
       </c>
       <c r="AR135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS135">
         <v>0</v>
       </c>
       <c r="AT135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU135">
         <v>1</v>
@@ -21349,58 +21349,58 @@
         <v>182</v>
       </c>
       <c r="E136" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F136" t="s">
         <v>377</v>
       </c>
       <c r="G136">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H136">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="I136">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J136">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K136">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L136">
-        <v>0.243</v>
+        <v>0.241</v>
       </c>
       <c r="M136">
-        <v>0.316</v>
+        <v>0.264</v>
       </c>
       <c r="N136">
-        <v>0.138</v>
+        <v>0.073</v>
       </c>
       <c r="O136">
-        <v>0.336</v>
+        <v>0.278</v>
       </c>
       <c r="P136">
-        <v>0.381</v>
+        <v>0.314</v>
       </c>
       <c r="Q136">
-        <v>0.718</v>
+        <v>0.592</v>
       </c>
       <c r="R136">
-        <v>14</v>
+        <v>12.9</v>
       </c>
       <c r="S136">
-        <v>12.1</v>
+        <v>4.1</v>
       </c>
       <c r="T136">
-        <v>43.2</v>
+        <v>53.4</v>
       </c>
       <c r="U136">
-        <v>38.1</v>
+        <v>35.6</v>
       </c>
       <c r="V136">
-        <v>28.8</v>
+        <v>24</v>
       </c>
       <c r="W136" t="s">
         <v>393</v>
@@ -21418,58 +21418,58 @@
         <v>393</v>
       </c>
       <c r="AB136" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC136">
         <v>12</v>
       </c>
       <c r="AD136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE136">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="AF136">
-        <v>0.436</v>
+        <v>0.192</v>
       </c>
       <c r="AG136">
-        <v>8.300000000000001</v>
+        <v>0</v>
       </c>
       <c r="AH136">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AI136">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="AJ136">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AK136">
-        <v>0.167</v>
+        <v>0.083</v>
       </c>
       <c r="AL136">
-        <v>8.029999999999999</v>
+        <v>4.96</v>
       </c>
       <c r="AM136">
-        <v>0.5710000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="AN136">
-        <v>0.286</v>
+        <v>0.2</v>
       </c>
       <c r="AO136">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AP136">
-        <v>0.286</v>
+        <v>0.2</v>
       </c>
       <c r="AQ136">
         <v>0</v>
       </c>
       <c r="AR136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT136">
         <v>0</v>
@@ -22377,7 +22377,7 @@
         <v>377</v>
       </c>
       <c r="G143">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H143">
         <v>184</v>
@@ -22669,7 +22669,7 @@
         <v>377</v>
       </c>
       <c r="G145">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H145">
         <v>143</v>
@@ -28071,7 +28071,7 @@
         <v>377</v>
       </c>
       <c r="G182">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H182">
         <v>118</v>
@@ -28211,58 +28211,58 @@
         <v>229</v>
       </c>
       <c r="E183" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F183" t="s">
         <v>377</v>
       </c>
       <c r="G183">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H183">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="I183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J183">
         <v>0</v>
       </c>
       <c r="K183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L183">
-        <v>0.259</v>
+        <v>0</v>
       </c>
       <c r="M183">
-        <v>0.315</v>
+        <v>0</v>
       </c>
       <c r="N183">
-        <v>0.08599999999999999</v>
+        <v>0</v>
       </c>
       <c r="O183">
-        <v>0.348</v>
+        <v>0</v>
       </c>
       <c r="P183">
-        <v>0.346</v>
+        <v>0</v>
       </c>
       <c r="Q183">
-        <v>0.694</v>
+        <v>0</v>
       </c>
       <c r="R183">
-        <v>17.2</v>
+        <v>33.3</v>
       </c>
       <c r="S183">
-        <v>8.6</v>
+        <v>0</v>
       </c>
       <c r="T183">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="U183">
-        <v>27.7</v>
+        <v>50</v>
       </c>
       <c r="V183">
-        <v>27.3</v>
+        <v>0</v>
       </c>
       <c r="W183" t="s">
         <v>399</v>
@@ -28280,55 +28280,55 @@
         <v>399</v>
       </c>
       <c r="AB183" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AC183">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AD183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE183">
-        <v>0.138</v>
+        <v>0.292</v>
       </c>
       <c r="AF183">
-        <v>0.224</v>
+        <v>0.413</v>
       </c>
       <c r="AG183">
-        <v>3.1</v>
+        <v>0</v>
       </c>
       <c r="AH183">
-        <v>0.138</v>
+        <v>0.208</v>
       </c>
       <c r="AI183">
-        <v>0.276</v>
+        <v>0.5</v>
       </c>
       <c r="AJ183">
-        <v>18.8</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="AK183">
-        <v>0.094</v>
+        <v>0.235</v>
       </c>
       <c r="AL183">
-        <v>4.36</v>
+        <v>6.16</v>
       </c>
       <c r="AM183">
-        <v>0.478</v>
+        <v>0.333</v>
       </c>
       <c r="AN183">
-        <v>0.391</v>
+        <v>0.381</v>
       </c>
       <c r="AO183">
-        <v>11.1</v>
+        <v>0</v>
       </c>
       <c r="AP183">
-        <v>0.304</v>
+        <v>0.182</v>
       </c>
       <c r="AQ183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS183">
         <v>1</v>
@@ -28363,52 +28363,52 @@
         <v>377</v>
       </c>
       <c r="G184">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H184">
-        <v>180</v>
+        <v>81</v>
       </c>
       <c r="I184">
         <v>1</v>
       </c>
       <c r="J184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K184">
         <v>0</v>
       </c>
       <c r="L184">
-        <v>0.261</v>
+        <v>0.259</v>
       </c>
       <c r="M184">
-        <v>0.284</v>
+        <v>0.315</v>
       </c>
       <c r="N184">
-        <v>0.083</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="O184">
-        <v>0.298</v>
+        <v>0.348</v>
       </c>
       <c r="P184">
-        <v>0.344</v>
+        <v>0.346</v>
       </c>
       <c r="Q184">
-        <v>0.643</v>
+        <v>0.694</v>
       </c>
       <c r="R184">
-        <v>24.6</v>
+        <v>17.2</v>
       </c>
       <c r="S184">
-        <v>5.2</v>
+        <v>8.6</v>
       </c>
       <c r="T184">
-        <v>54.5</v>
+        <v>60</v>
       </c>
       <c r="U184">
-        <v>23.1</v>
+        <v>27.7</v>
       </c>
       <c r="V184">
-        <v>31.3</v>
+        <v>27.3</v>
       </c>
       <c r="W184" t="s">
         <v>399</v>
@@ -28471,10 +28471,10 @@
         <v>0.304</v>
       </c>
       <c r="AQ184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR184">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS184">
         <v>1</v>
@@ -28503,58 +28503,58 @@
         <v>231</v>
       </c>
       <c r="E185" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F185" t="s">
         <v>377</v>
       </c>
       <c r="G185">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H185">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="I185">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J185">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K185">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L185">
-        <v>0.256</v>
+        <v>0.261</v>
       </c>
       <c r="M185">
-        <v>0.337</v>
+        <v>0.284</v>
       </c>
       <c r="N185">
-        <v>0.188</v>
+        <v>0.083</v>
       </c>
       <c r="O185">
-        <v>0.33</v>
+        <v>0.298</v>
       </c>
       <c r="P185">
-        <v>0.444</v>
+        <v>0.344</v>
       </c>
       <c r="Q185">
-        <v>0.775</v>
+        <v>0.643</v>
       </c>
       <c r="R185">
-        <v>28.1</v>
+        <v>24.6</v>
       </c>
       <c r="S185">
-        <v>10.2</v>
+        <v>5.2</v>
       </c>
       <c r="T185">
-        <v>46.5</v>
+        <v>54.5</v>
       </c>
       <c r="U185">
-        <v>33.1</v>
+        <v>23.1</v>
       </c>
       <c r="V185">
-        <v>42</v>
+        <v>31.3</v>
       </c>
       <c r="W185" t="s">
         <v>399</v>
@@ -28572,55 +28572,55 @@
         <v>399</v>
       </c>
       <c r="AB185" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC185">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AD185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE185">
-        <v>0.292</v>
+        <v>0.138</v>
       </c>
       <c r="AF185">
-        <v>0.413</v>
+        <v>0.224</v>
       </c>
       <c r="AG185">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="AH185">
-        <v>0.208</v>
+        <v>0.138</v>
       </c>
       <c r="AI185">
-        <v>0.5</v>
+        <v>0.276</v>
       </c>
       <c r="AJ185">
-        <v>8.800000000000001</v>
+        <v>18.8</v>
       </c>
       <c r="AK185">
-        <v>0.235</v>
+        <v>0.094</v>
       </c>
       <c r="AL185">
-        <v>6.16</v>
+        <v>4.36</v>
       </c>
       <c r="AM185">
-        <v>0.333</v>
+        <v>0.478</v>
       </c>
       <c r="AN185">
-        <v>0.381</v>
+        <v>0.391</v>
       </c>
       <c r="AO185">
-        <v>0</v>
+        <v>11.1</v>
       </c>
       <c r="AP185">
-        <v>0.182</v>
+        <v>0.304</v>
       </c>
       <c r="AQ185">
         <v>1</v>
       </c>
       <c r="AR185">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS185">
         <v>1</v>
@@ -28632,7 +28632,7 @@
         <v>0</v>
       </c>
       <c r="AV185">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:48">
@@ -28649,28 +28649,28 @@
         <v>232</v>
       </c>
       <c r="E186" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F186" t="s">
         <v>377</v>
       </c>
       <c r="G186">
+        <v>3</v>
+      </c>
+      <c r="H186">
+        <v>207</v>
+      </c>
+      <c r="I186">
+        <v>9</v>
+      </c>
+      <c r="J186">
         <v>2</v>
       </c>
-      <c r="H186">
-        <v>240</v>
-      </c>
-      <c r="I186">
-        <v>7</v>
-      </c>
-      <c r="J186">
-        <v>3</v>
-      </c>
       <c r="K186">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L186">
-        <v>0.288</v>
+        <v>0.256</v>
       </c>
       <c r="M186">
         <v>0.337</v>
@@ -28679,28 +28679,28 @@
         <v>0.188</v>
       </c>
       <c r="O186">
-        <v>0.309</v>
+        <v>0.33</v>
       </c>
       <c r="P186">
-        <v>0.475</v>
+        <v>0.444</v>
       </c>
       <c r="Q186">
-        <v>0.784</v>
+        <v>0.775</v>
       </c>
       <c r="R186">
-        <v>26.6</v>
+        <v>28.1</v>
       </c>
       <c r="S186">
-        <v>2.4</v>
+        <v>10.2</v>
       </c>
       <c r="T186">
-        <v>31.2</v>
+        <v>46.5</v>
       </c>
       <c r="U186">
-        <v>45.1</v>
+        <v>33.1</v>
       </c>
       <c r="V186">
-        <v>32.2</v>
+        <v>42</v>
       </c>
       <c r="W186" t="s">
         <v>399</v>
@@ -28718,58 +28718,58 @@
         <v>399</v>
       </c>
       <c r="AB186" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AC186">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AD186">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE186">
-        <v>0.138</v>
+        <v>0.292</v>
       </c>
       <c r="AF186">
-        <v>0.224</v>
+        <v>0.413</v>
       </c>
       <c r="AG186">
-        <v>3.1</v>
+        <v>0</v>
       </c>
       <c r="AH186">
-        <v>0.138</v>
+        <v>0.208</v>
       </c>
       <c r="AI186">
-        <v>0.276</v>
+        <v>0.5</v>
       </c>
       <c r="AJ186">
-        <v>18.8</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="AK186">
-        <v>0.094</v>
+        <v>0.235</v>
       </c>
       <c r="AL186">
-        <v>4.36</v>
+        <v>6.16</v>
       </c>
       <c r="AM186">
-        <v>0.478</v>
+        <v>0.333</v>
       </c>
       <c r="AN186">
-        <v>0.391</v>
+        <v>0.381</v>
       </c>
       <c r="AO186">
-        <v>11.1</v>
+        <v>0</v>
       </c>
       <c r="AP186">
-        <v>0.304</v>
+        <v>0.182</v>
       </c>
       <c r="AQ186">
         <v>1</v>
       </c>
       <c r="AR186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT186">
         <v>0</v>
@@ -28778,7 +28778,7 @@
         <v>0</v>
       </c>
       <c r="AV186">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:48">
@@ -28801,52 +28801,52 @@
         <v>377</v>
       </c>
       <c r="G187">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H187">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="I187">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J187">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="K187">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L187">
-        <v>0.26</v>
+        <v>0.288</v>
       </c>
       <c r="M187">
-        <v>0.314</v>
+        <v>0.337</v>
       </c>
       <c r="N187">
-        <v>0.135</v>
+        <v>0.188</v>
       </c>
       <c r="O187">
-        <v>0.321</v>
+        <v>0.309</v>
       </c>
       <c r="P187">
-        <v>0.395</v>
+        <v>0.475</v>
       </c>
       <c r="Q187">
-        <v>0.716</v>
+        <v>0.784</v>
       </c>
       <c r="R187">
-        <v>27.6</v>
+        <v>26.6</v>
       </c>
       <c r="S187">
-        <v>7.8</v>
+        <v>2.4</v>
       </c>
       <c r="T187">
-        <v>48.7</v>
+        <v>31.2</v>
       </c>
       <c r="U187">
-        <v>34.9</v>
+        <v>45.1</v>
       </c>
       <c r="V187">
-        <v>29.7</v>
+        <v>32.2</v>
       </c>
       <c r="W187" t="s">
         <v>399</v>
@@ -28915,7 +28915,7 @@
         <v>0</v>
       </c>
       <c r="AS187">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT187">
         <v>0</v>
@@ -28941,58 +28941,58 @@
         <v>234</v>
       </c>
       <c r="E188" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F188" t="s">
         <v>377</v>
       </c>
       <c r="G188">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H188">
-        <v>80</v>
+        <v>215</v>
       </c>
       <c r="I188">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J188">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="K188">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L188">
-        <v>0.213</v>
+        <v>0.26</v>
       </c>
       <c r="M188">
-        <v>0.306</v>
+        <v>0.314</v>
       </c>
       <c r="N188">
-        <v>0.25</v>
+        <v>0.135</v>
       </c>
       <c r="O188">
-        <v>0.256</v>
+        <v>0.321</v>
       </c>
       <c r="P188">
-        <v>0.463</v>
+        <v>0.395</v>
       </c>
       <c r="Q188">
-        <v>0.718</v>
+        <v>0.716</v>
       </c>
       <c r="R188">
-        <v>36</v>
+        <v>27.6</v>
       </c>
       <c r="S188">
-        <v>4.7</v>
+        <v>7.8</v>
       </c>
       <c r="T188">
-        <v>34</v>
+        <v>48.7</v>
       </c>
       <c r="U188">
-        <v>46</v>
+        <v>34.9</v>
       </c>
       <c r="V188">
-        <v>42</v>
+        <v>29.7</v>
       </c>
       <c r="W188" t="s">
         <v>399</v>
@@ -29010,49 +29010,49 @@
         <v>399</v>
       </c>
       <c r="AB188" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC188">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AD188">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE188">
-        <v>0.292</v>
+        <v>0.138</v>
       </c>
       <c r="AF188">
-        <v>0.413</v>
+        <v>0.224</v>
       </c>
       <c r="AG188">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="AH188">
-        <v>0.208</v>
+        <v>0.138</v>
       </c>
       <c r="AI188">
-        <v>0.5</v>
+        <v>0.276</v>
       </c>
       <c r="AJ188">
-        <v>8.800000000000001</v>
+        <v>18.8</v>
       </c>
       <c r="AK188">
-        <v>0.235</v>
+        <v>0.094</v>
       </c>
       <c r="AL188">
-        <v>6.16</v>
+        <v>4.36</v>
       </c>
       <c r="AM188">
-        <v>0.333</v>
+        <v>0.478</v>
       </c>
       <c r="AN188">
-        <v>0.381</v>
+        <v>0.391</v>
       </c>
       <c r="AO188">
-        <v>0</v>
+        <v>11.1</v>
       </c>
       <c r="AP188">
-        <v>0.182</v>
+        <v>0.304</v>
       </c>
       <c r="AQ188">
         <v>1</v>
@@ -29061,16 +29061,16 @@
         <v>0</v>
       </c>
       <c r="AS188">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT188">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU188">
         <v>0</v>
       </c>
       <c r="AV188">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:48">
@@ -29087,7 +29087,7 @@
         <v>235</v>
       </c>
       <c r="E189" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F189" t="s">
         <v>377</v>
@@ -29096,49 +29096,49 @@
         <v>5</v>
       </c>
       <c r="H189">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I189">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J189">
         <v>1</v>
       </c>
       <c r="K189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L189">
-        <v>0.184</v>
+        <v>0.213</v>
       </c>
       <c r="M189">
-        <v>0.271</v>
+        <v>0.306</v>
       </c>
       <c r="N189">
-        <v>0.115</v>
+        <v>0.25</v>
       </c>
       <c r="O189">
-        <v>0.301</v>
+        <v>0.256</v>
       </c>
       <c r="P189">
-        <v>0.299</v>
+        <v>0.463</v>
       </c>
       <c r="Q189">
-        <v>0.6</v>
+        <v>0.718</v>
       </c>
       <c r="R189">
-        <v>31.1</v>
+        <v>36</v>
       </c>
       <c r="S189">
-        <v>14.6</v>
+        <v>4.7</v>
       </c>
       <c r="T189">
-        <v>42.9</v>
+        <v>34</v>
       </c>
       <c r="U189">
-        <v>35.7</v>
+        <v>46</v>
       </c>
       <c r="V189">
-        <v>33.9</v>
+        <v>42</v>
       </c>
       <c r="W189" t="s">
         <v>399</v>
@@ -29204,19 +29204,19 @@
         <v>1</v>
       </c>
       <c r="AR189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS189">
         <v>0</v>
       </c>
       <c r="AT189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU189">
         <v>0</v>
       </c>
       <c r="AV189">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:48">
@@ -29233,19 +29233,19 @@
         <v>236</v>
       </c>
       <c r="E190" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F190" t="s">
         <v>377</v>
       </c>
       <c r="G190">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H190">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="I190">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J190">
         <v>1</v>
@@ -29254,37 +29254,37 @@
         <v>1</v>
       </c>
       <c r="L190">
-        <v>0.174</v>
+        <v>0.184</v>
       </c>
       <c r="M190">
-        <v>0.243</v>
+        <v>0.271</v>
       </c>
       <c r="N190">
-        <v>0.159</v>
+        <v>0.115</v>
       </c>
       <c r="O190">
-        <v>0.219</v>
+        <v>0.301</v>
       </c>
       <c r="P190">
-        <v>0.333</v>
+        <v>0.299</v>
       </c>
       <c r="Q190">
-        <v>0.553</v>
+        <v>0.6</v>
       </c>
       <c r="R190">
-        <v>30.1</v>
+        <v>31.1</v>
       </c>
       <c r="S190">
-        <v>4.1</v>
+        <v>14.6</v>
       </c>
       <c r="T190">
-        <v>38.3</v>
+        <v>42.9</v>
       </c>
       <c r="U190">
-        <v>48.9</v>
+        <v>35.7</v>
       </c>
       <c r="V190">
-        <v>31.9</v>
+        <v>33.9</v>
       </c>
       <c r="W190" t="s">
         <v>399</v>
@@ -29302,55 +29302,55 @@
         <v>399</v>
       </c>
       <c r="AB190" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AC190">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AD190">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE190">
-        <v>0.138</v>
+        <v>0.292</v>
       </c>
       <c r="AF190">
-        <v>0.224</v>
+        <v>0.413</v>
       </c>
       <c r="AG190">
-        <v>3.1</v>
+        <v>0</v>
       </c>
       <c r="AH190">
-        <v>0.138</v>
+        <v>0.208</v>
       </c>
       <c r="AI190">
-        <v>0.276</v>
+        <v>0.5</v>
       </c>
       <c r="AJ190">
-        <v>18.8</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="AK190">
-        <v>0.094</v>
+        <v>0.235</v>
       </c>
       <c r="AL190">
-        <v>4.36</v>
+        <v>6.16</v>
       </c>
       <c r="AM190">
-        <v>0.478</v>
+        <v>0.333</v>
       </c>
       <c r="AN190">
-        <v>0.391</v>
+        <v>0.381</v>
       </c>
       <c r="AO190">
-        <v>11.1</v>
+        <v>0</v>
       </c>
       <c r="AP190">
-        <v>0.304</v>
+        <v>0.182</v>
       </c>
       <c r="AQ190">
         <v>1</v>
       </c>
       <c r="AR190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS190">
         <v>0</v>
@@ -33327,7 +33327,7 @@
         <v>377</v>
       </c>
       <c r="G218">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H218">
         <v>140</v>
@@ -33911,7 +33911,7 @@
         <v>377</v>
       </c>
       <c r="G222">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H222">
         <v>94</v>
@@ -34051,58 +34051,58 @@
         <v>269</v>
       </c>
       <c r="E223" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F223" t="s">
         <v>377</v>
       </c>
       <c r="G223">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H223">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="I223">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J223">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K223">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L223">
-        <v>0.244</v>
+        <v>0.318</v>
       </c>
       <c r="M223">
-        <v>0.324</v>
+        <v>0.356</v>
       </c>
       <c r="N223">
-        <v>0.228</v>
+        <v>0.136</v>
       </c>
       <c r="O223">
-        <v>0.289</v>
+        <v>0.361</v>
       </c>
       <c r="P223">
-        <v>0.472</v>
+        <v>0.455</v>
       </c>
       <c r="Q223">
-        <v>0.76</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="R223">
-        <v>24.4</v>
+        <v>19.4</v>
       </c>
       <c r="S223">
-        <v>6.7</v>
+        <v>2.8</v>
       </c>
       <c r="T223">
-        <v>30.4</v>
+        <v>41.7</v>
       </c>
       <c r="U223">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="V223">
-        <v>37.6</v>
+        <v>19.8</v>
       </c>
       <c r="W223" t="s">
         <v>403</v>
@@ -34120,52 +34120,52 @@
         <v>415</v>
       </c>
       <c r="AB223" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC223">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="AD223">
         <v>5</v>
       </c>
       <c r="AE223">
-        <v>0.474</v>
+        <v>0.261</v>
       </c>
       <c r="AF223">
-        <v>0.532</v>
+        <v>0.325</v>
       </c>
       <c r="AG223">
-        <v>5.8</v>
+        <v>3.9</v>
       </c>
       <c r="AH223">
-        <v>0.244</v>
+        <v>0.201</v>
       </c>
       <c r="AI223">
-        <v>0.718</v>
+        <v>0.462</v>
       </c>
       <c r="AJ223">
-        <v>9.300000000000001</v>
+        <v>18.1</v>
       </c>
       <c r="AK223">
-        <v>0.081</v>
+        <v>0.039</v>
       </c>
       <c r="AL223">
-        <v>8.02</v>
+        <v>4.29</v>
       </c>
       <c r="AM223">
-        <v>0.429</v>
+        <v>0.402</v>
       </c>
       <c r="AN223">
-        <v>0.271</v>
+        <v>0.433</v>
       </c>
       <c r="AO223">
-        <v>26.3</v>
+        <v>11.9</v>
       </c>
       <c r="AP223">
-        <v>0.314</v>
+        <v>0.337</v>
       </c>
       <c r="AQ223">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR223">
         <v>0</v>
@@ -34174,13 +34174,13 @@
         <v>0</v>
       </c>
       <c r="AT223">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU223">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV223">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:48">
@@ -34197,58 +34197,58 @@
         <v>270</v>
       </c>
       <c r="E224" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F224" t="s">
         <v>377</v>
       </c>
       <c r="G224">
+        <v>2</v>
+      </c>
+      <c r="H224">
+        <v>129</v>
+      </c>
+      <c r="I224">
         <v>5</v>
       </c>
-      <c r="H224">
-        <v>132</v>
-      </c>
-      <c r="I224">
-        <v>4</v>
-      </c>
       <c r="J224">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="K224">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L224">
-        <v>0.318</v>
+        <v>0.295</v>
       </c>
       <c r="M224">
-        <v>0.356</v>
+        <v>0.364</v>
       </c>
       <c r="N224">
-        <v>0.136</v>
+        <v>0.194</v>
       </c>
       <c r="O224">
-        <v>0.361</v>
+        <v>0.35</v>
       </c>
       <c r="P224">
-        <v>0.455</v>
+        <v>0.488</v>
       </c>
       <c r="Q224">
-        <v>0.8159999999999999</v>
+        <v>0.838</v>
       </c>
       <c r="R224">
-        <v>19.4</v>
+        <v>22.9</v>
       </c>
       <c r="S224">
-        <v>2.8</v>
+        <v>7.1</v>
       </c>
       <c r="T224">
-        <v>41.7</v>
+        <v>35.1</v>
       </c>
       <c r="U224">
-        <v>35</v>
+        <v>42.6</v>
       </c>
       <c r="V224">
-        <v>19.8</v>
+        <v>23.7</v>
       </c>
       <c r="W224" t="s">
         <v>403</v>
@@ -34266,52 +34266,52 @@
         <v>415</v>
       </c>
       <c r="AB224" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AC224">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="AD224">
         <v>5</v>
       </c>
       <c r="AE224">
-        <v>0.261</v>
+        <v>0.474</v>
       </c>
       <c r="AF224">
-        <v>0.325</v>
+        <v>0.532</v>
       </c>
       <c r="AG224">
-        <v>3.9</v>
+        <v>5.8</v>
       </c>
       <c r="AH224">
-        <v>0.201</v>
+        <v>0.244</v>
       </c>
       <c r="AI224">
-        <v>0.462</v>
+        <v>0.718</v>
       </c>
       <c r="AJ224">
-        <v>18.1</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="AK224">
-        <v>0.039</v>
+        <v>0.081</v>
       </c>
       <c r="AL224">
-        <v>4.29</v>
+        <v>8.02</v>
       </c>
       <c r="AM224">
-        <v>0.402</v>
+        <v>0.429</v>
       </c>
       <c r="AN224">
-        <v>0.433</v>
+        <v>0.271</v>
       </c>
       <c r="AO224">
-        <v>11.9</v>
+        <v>26.3</v>
       </c>
       <c r="AP224">
-        <v>0.337</v>
+        <v>0.314</v>
       </c>
       <c r="AQ224">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR224">
         <v>0</v>
@@ -34349,52 +34349,52 @@
         <v>377</v>
       </c>
       <c r="G225">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H225">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="I225">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J225">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="K225">
         <v>1</v>
       </c>
       <c r="L225">
-        <v>0.295</v>
+        <v>0.277</v>
       </c>
       <c r="M225">
-        <v>0.364</v>
+        <v>0.368</v>
       </c>
       <c r="N225">
-        <v>0.194</v>
+        <v>0.232</v>
       </c>
       <c r="O225">
-        <v>0.35</v>
+        <v>0.347</v>
       </c>
       <c r="P225">
-        <v>0.488</v>
+        <v>0.51</v>
       </c>
       <c r="Q225">
-        <v>0.838</v>
+        <v>0.856</v>
       </c>
       <c r="R225">
-        <v>22.9</v>
+        <v>25.4</v>
       </c>
       <c r="S225">
-        <v>7.1</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="T225">
-        <v>35.1</v>
+        <v>36.6</v>
       </c>
       <c r="U225">
-        <v>42.6</v>
+        <v>49.1</v>
       </c>
       <c r="V225">
-        <v>23.7</v>
+        <v>33.9</v>
       </c>
       <c r="W225" t="s">
         <v>403</v>
@@ -34460,13 +34460,13 @@
         <v>1</v>
       </c>
       <c r="AR225">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS225">
         <v>0</v>
       </c>
       <c r="AT225">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU225">
         <v>1</v>
@@ -34489,58 +34489,58 @@
         <v>272</v>
       </c>
       <c r="E226" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F226" t="s">
         <v>377</v>
       </c>
       <c r="G226">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H226">
-        <v>155</v>
+        <v>202</v>
       </c>
       <c r="I226">
         <v>6</v>
       </c>
       <c r="J226">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K226">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L226">
-        <v>0.277</v>
+        <v>0.228</v>
       </c>
       <c r="M226">
-        <v>0.368</v>
+        <v>0.265</v>
       </c>
       <c r="N226">
-        <v>0.232</v>
+        <v>0.134</v>
       </c>
       <c r="O226">
-        <v>0.347</v>
+        <v>0.25</v>
       </c>
       <c r="P226">
-        <v>0.51</v>
+        <v>0.361</v>
       </c>
       <c r="Q226">
-        <v>0.856</v>
+        <v>0.611</v>
       </c>
       <c r="R226">
-        <v>25.4</v>
+        <v>26.3</v>
       </c>
       <c r="S226">
-        <v>9.800000000000001</v>
+        <v>2.3</v>
       </c>
       <c r="T226">
-        <v>36.6</v>
+        <v>38.1</v>
       </c>
       <c r="U226">
-        <v>49.1</v>
+        <v>39.5</v>
       </c>
       <c r="V226">
-        <v>33.9</v>
+        <v>20.7</v>
       </c>
       <c r="W226" t="s">
         <v>403</v>
@@ -34558,64 +34558,64 @@
         <v>415</v>
       </c>
       <c r="AB226" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC226">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="AD226">
         <v>5</v>
       </c>
       <c r="AE226">
-        <v>0.474</v>
+        <v>0.261</v>
       </c>
       <c r="AF226">
-        <v>0.532</v>
+        <v>0.325</v>
       </c>
       <c r="AG226">
-        <v>5.8</v>
+        <v>3.9</v>
       </c>
       <c r="AH226">
-        <v>0.244</v>
+        <v>0.201</v>
       </c>
       <c r="AI226">
-        <v>0.718</v>
+        <v>0.462</v>
       </c>
       <c r="AJ226">
-        <v>9.300000000000001</v>
+        <v>18.1</v>
       </c>
       <c r="AK226">
-        <v>0.081</v>
+        <v>0.039</v>
       </c>
       <c r="AL226">
-        <v>8.02</v>
+        <v>4.29</v>
       </c>
       <c r="AM226">
-        <v>0.429</v>
+        <v>0.402</v>
       </c>
       <c r="AN226">
-        <v>0.271</v>
+        <v>0.433</v>
       </c>
       <c r="AO226">
-        <v>26.3</v>
+        <v>11.9</v>
       </c>
       <c r="AP226">
-        <v>0.314</v>
+        <v>0.337</v>
       </c>
       <c r="AQ226">
         <v>1</v>
       </c>
       <c r="AR226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS226">
         <v>0</v>
       </c>
       <c r="AT226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV226">
         <v>0</v>

</xml_diff>

<commit_message>
Updating Daily Files for June 3
</commit_message>
<xml_diff>
--- a/assets/Combined_Daily_Data.xlsx
+++ b/assets/Combined_Daily_Data.xlsx
@@ -11168,7 +11168,7 @@
         <v>0.7140000000000001</v>
       </c>
       <c r="AR66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS66">
         <v>1</v>
@@ -13904,7 +13904,7 @@
         <v>0.2822190476190476</v>
       </c>
       <c r="AR84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS84">
         <v>1</v>
@@ -15728,7 +15728,7 @@
         <v>0.2888729281767956</v>
       </c>
       <c r="AR96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS96">
         <v>0</v>
@@ -16488,7 +16488,7 @@
         <v>0.3359767441860465</v>
       </c>
       <c r="AR101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS101">
         <v>0</v>
@@ -18893,7 +18893,7 @@
         <v>0.462</v>
       </c>
       <c r="AR117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS117">
         <v>0</v>

</xml_diff>